<commit_message>
lots of little updates...see TODO/DONE..also work more on npc target stuff
</commit_message>
<xml_diff>
--- a/AncientWarfare/project_resources/45deg angle vel calc.xlsx
+++ b/AncientWarfare/project_resources/45deg angle vel calc.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="11505" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="11505"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="calcAngle" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>g</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>sqrt</t>
+  </si>
+  <si>
+    <t>xxxx</t>
   </si>
 </sst>
 </file>
@@ -82,12 +85,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,9 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +416,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>99.896789999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>B5*B5</f>
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>B5*B5*B5*B5</f>
+        <v>1185921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <f>B2*B2</f>
+        <v>9979.3686523040997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <f>SQRT(B10-B1*(B1*B11+2*B3*B9))</f>
+        <v>109.01229490290181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <f>B9+B12</f>
+        <v>1198.0122949029019</v>
+      </c>
+      <c r="B14">
+        <f>A14/ (B1*B2)</f>
+        <v>1.2224771058818389</v>
+      </c>
+      <c r="C14">
+        <f>ATAN(B14)</f>
+        <v>0.88516900894638439</v>
+      </c>
+      <c r="D14">
+        <f>DEGREES(C14)</f>
+        <v>50.716448368405636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <f>B9-B12</f>
+        <v>979.98770509709823</v>
+      </c>
+      <c r="B15">
+        <f>A15/(B1*B2)</f>
+        <v>1.000000199183251</v>
+      </c>
+      <c r="C15">
+        <f>ATAN(B15)</f>
+        <v>0.7853982629890639</v>
+      </c>
+      <c r="D15" s="2">
+        <f>DEGREES(C15)</f>
+        <v>45.000005706179252</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -518,12 +662,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -615,128 +759,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>9.81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>33.014282000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <f>B5*B5</f>
-        <v>1089.9428159755241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <f>B5*B5*B5*B5</f>
-        <v>1187975.3420966552</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <f>B2*B2</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <f>SQRT(B10-B1*(B1*B11+2*B3*B9))</f>
-        <v>108.47839232887438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <f>B9+B12</f>
-        <v>1198.4212083043985</v>
-      </c>
-      <c r="B14">
-        <f>A14/ (B1*B2)</f>
-        <v>1.2216322204937804</v>
-      </c>
-      <c r="C14">
-        <f>ATAN(B14)</f>
-        <v>0.88483016261103575</v>
-      </c>
-      <c r="D14">
-        <f>DEGREES(C14)</f>
-        <v>50.697033903486684</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <f>B9-B12</f>
-        <v>981.46442364664972</v>
-      </c>
-      <c r="B15">
-        <f>A15/(B1*B2)</f>
-        <v>1.0004734186000508</v>
-      </c>
-      <c r="C15">
-        <f>ATAN(B15)</f>
-        <v>0.78563481667502311</v>
-      </c>
-      <c r="D15">
-        <f>DEGREES(C15)</f>
-        <v>45.013559234012973</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>